<commit_message>
glasser region descriptions, meta-analysis agency update, Kraynak 2018 foci added
</commit_message>
<xml_diff>
--- a/CANlab_Meta_analysis_maps/2011_Agency_Meta_analysis/Agency_meta_analysis_database.xlsx
+++ b/CANlab_Meta_analysis_maps/2011_Agency_Meta_analysis/Agency_meta_analysis_database.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torwager/Documents/GitHub/Neuroimaging_Pattern_Masks/CANlab_Meta_analysis_maps/2011_Agency_Meta_analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32653C4-36D5-F04B-B59B-1CFD14CA90D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="27520" windowHeight="26840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="19440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130407"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -30,24 +36,15 @@
     <t>z</t>
   </si>
   <si>
-    <t>Study</t>
-  </si>
-  <si>
     <t>Contrast</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>Original_Space</t>
-  </si>
-  <si>
     <t>MNI</t>
   </si>
   <si>
-    <t>TAL</t>
-  </si>
-  <si>
     <t>Chaminade_&amp;_Decety,_2002</t>
   </si>
   <si>
@@ -100,13 +97,22 @@
   </si>
   <si>
     <t>Farrer_2008_Study_2</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>CoordSys</t>
+  </si>
+  <si>
+    <t>T88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -144,6 +150,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -466,24 +480,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -494,19 +508,19 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>44</v>
       </c>
@@ -517,7 +531,7 @@
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -526,10 +540,10 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>32</v>
       </c>
@@ -540,7 +554,7 @@
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -549,10 +563,10 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>-50</v>
       </c>
@@ -563,7 +577,7 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -572,10 +586,10 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>58</v>
       </c>
@@ -586,7 +600,7 @@
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -595,10 +609,10 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>44</v>
       </c>
@@ -609,7 +623,7 @@
         <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -618,10 +632,10 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>-54</v>
       </c>
@@ -632,7 +646,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -641,10 +655,10 @@
         <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>54</v>
       </c>
@@ -655,7 +669,7 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -664,10 +678,10 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>-64</v>
       </c>
@@ -678,7 +692,7 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -687,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>56</v>
       </c>
@@ -701,7 +715,7 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -710,10 +724,10 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>56</v>
       </c>
@@ -724,7 +738,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -733,10 +747,10 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>-48</v>
       </c>
@@ -747,7 +761,7 @@
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -756,10 +770,10 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>44</v>
       </c>
@@ -770,7 +784,7 @@
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -779,10 +793,10 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>48</v>
       </c>
@@ -793,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -802,10 +816,10 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>44</v>
       </c>
@@ -816,7 +830,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>8</v>
@@ -825,10 +839,10 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>50</v>
       </c>
@@ -839,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>8</v>
@@ -848,10 +862,10 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>-59</v>
       </c>
@@ -862,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E18">
         <v>9</v>
@@ -871,10 +885,10 @@
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>-50</v>
       </c>
@@ -885,7 +899,7 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E19">
         <v>9</v>
@@ -894,10 +908,10 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>62</v>
       </c>
@@ -908,7 +922,7 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <v>9</v>
@@ -917,10 +931,10 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>53</v>
       </c>
@@ -931,7 +945,7 @@
         <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E21">
         <v>9</v>
@@ -940,10 +954,10 @@
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>59</v>
       </c>
@@ -954,7 +968,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -963,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>55</v>
       </c>
@@ -977,7 +991,7 @@
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -986,10 +1000,10 @@
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>-40</v>
       </c>
@@ -1000,7 +1014,7 @@
         <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1009,10 +1023,10 @@
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>60</v>
       </c>
@@ -1023,7 +1037,7 @@
         <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E25">
         <v>11</v>
@@ -1032,10 +1046,10 @@
         <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>-42</v>
       </c>
@@ -1046,7 +1060,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26">
         <v>12</v>
@@ -1055,10 +1069,10 @@
         <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>-54</v>
       </c>
@@ -1069,7 +1083,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E27">
         <v>12</v>
@@ -1078,10 +1092,10 @@
         <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>54</v>
       </c>
@@ -1092,7 +1106,7 @@
         <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E28">
         <v>12</v>
@@ -1101,10 +1115,10 @@
         <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>-40</v>
       </c>
@@ -1115,7 +1129,7 @@
         <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E29">
         <v>13</v>
@@ -1124,10 +1138,10 @@
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>-48</v>
       </c>
@@ -1138,7 +1152,7 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E30">
         <v>13</v>
@@ -1147,10 +1161,10 @@
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>44</v>
       </c>
@@ -1161,7 +1175,7 @@
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E31">
         <v>13</v>
@@ -1170,10 +1184,10 @@
         <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>-48</v>
       </c>
@@ -1184,7 +1198,7 @@
         <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E32">
         <v>14</v>
@@ -1193,10 +1207,10 @@
         <v>18</v>
       </c>
       <c r="G32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>58</v>
       </c>
@@ -1207,7 +1221,7 @@
         <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E33">
         <v>14</v>
@@ -1216,10 +1230,10 @@
         <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>-49</v>
       </c>
@@ -1230,7 +1244,7 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E34">
         <v>15</v>
@@ -1239,10 +1253,10 @@
         <v>18</v>
       </c>
       <c r="G34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>54</v>
       </c>
@@ -1253,7 +1267,7 @@
         <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E35">
         <v>15</v>
@@ -1262,10 +1276,10 @@
         <v>18</v>
       </c>
       <c r="G35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>62</v>
       </c>
@@ -1276,7 +1290,7 @@
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E36">
         <v>16</v>
@@ -1285,10 +1299,10 @@
         <v>20</v>
       </c>
       <c r="G36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>58</v>
       </c>
@@ -1299,7 +1313,7 @@
         <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E37">
         <v>16</v>
@@ -1308,10 +1322,10 @@
         <v>20</v>
       </c>
       <c r="G37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>45</v>
       </c>
@@ -1322,7 +1336,7 @@
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E38">
         <v>16</v>
@@ -1331,10 +1345,10 @@
         <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>64</v>
       </c>
@@ -1345,7 +1359,7 @@
         <v>40</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E39">
         <v>16</v>
@@ -1354,10 +1368,10 @@
         <v>20</v>
       </c>
       <c r="G39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>-52</v>
       </c>
@@ -1368,7 +1382,7 @@
         <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E40">
         <v>16</v>
@@ -1377,10 +1391,10 @@
         <v>20</v>
       </c>
       <c r="G40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1391,7 +1405,7 @@
         <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E41">
         <v>16</v>
@@ -1400,10 +1414,10 @@
         <v>20</v>
       </c>
       <c r="G41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>56</v>
       </c>
@@ -1414,7 +1428,7 @@
         <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E42">
         <v>16</v>
@@ -1423,10 +1437,10 @@
         <v>20</v>
       </c>
       <c r="G42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>52</v>
       </c>
@@ -1437,7 +1451,7 @@
         <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E43">
         <v>16</v>
@@ -1446,10 +1460,10 @@
         <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>52</v>
       </c>
@@ -1460,7 +1474,7 @@
         <v>56</v>
       </c>
       <c r="D44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E44">
         <v>16</v>
@@ -1469,10 +1483,10 @@
         <v>20</v>
       </c>
       <c r="G44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>-46</v>
       </c>
@@ -1483,7 +1497,7 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E45">
         <v>16</v>
@@ -1492,10 +1506,10 @@
         <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>40</v>
       </c>
@@ -1506,7 +1520,7 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E46">
         <v>17</v>
@@ -1515,10 +1529,10 @@
         <v>19</v>
       </c>
       <c r="G46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>52</v>
       </c>
@@ -1529,7 +1543,7 @@
         <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E47">
         <v>17</v>
@@ -1538,10 +1552,10 @@
         <v>19</v>
       </c>
       <c r="G47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>52</v>
       </c>
@@ -1552,7 +1566,7 @@
         <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E48">
         <v>18</v>
@@ -1561,7 +1575,7 @@
         <v>28</v>
       </c>
       <c r="G48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>